<commit_message>
Update Laundry Website Data Dictionary.xlsx
Added all database variables
</commit_message>
<xml_diff>
--- a/Documentation/Laundry Website Data Dictionary.xlsx
+++ b/Documentation/Laundry Website Data Dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Andres Library\Cloud Documents\Kelvin's Documents\CSC 350\GitHub\BMCC_CSC350_SP21_E\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AED36E0-253C-4A89-8F59-B3B97632D09F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6588EA7-519F-4402-AECA-A0D2E746E6E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="-3120" windowWidth="16440" windowHeight="28440" xr2:uid="{07EEDACD-45F9-4513-A15E-788DF889D03E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>DATA DICTIONARY</t>
   </si>
@@ -102,9 +102,6 @@
     <t>userid</t>
   </si>
   <si>
-    <t>varchar</t>
-  </si>
-  <si>
     <t>No spaces, pre-defined</t>
   </si>
   <si>
@@ -118,6 +115,21 @@
   </si>
   <si>
     <t>P</t>
+  </si>
+  <si>
+    <t>week_day</t>
+  </si>
+  <si>
+    <t>slot</t>
+  </si>
+  <si>
+    <t>varchar(20)</t>
+  </si>
+  <si>
+    <t>Must be 1-7</t>
+  </si>
+  <si>
+    <t>Must be 1-8</t>
   </si>
 </sst>
 </file>
@@ -717,7 +729,7 @@
   <dimension ref="B2:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,53 +832,69 @@
     </row>
     <row r="12" spans="2:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F12" s="2">
         <v>20</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="7"/>
       <c r="C13" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F13" s="2">
         <v>16</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="7"/>
-      <c r="C14" s="2"/>
+      <c r="C14" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="8"/>
+      <c r="E14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="2">
+        <v>1</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="15" spans="2:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="7"/>
-      <c r="C15" s="2"/>
+      <c r="C15" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="8"/>
+      <c r="E15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="16" spans="2:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="7"/>
@@ -1042,12 +1070,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AA7C269EC0EF9C4BBEE1AE4ED895DE9E" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="871a8ee7b9883bca90c28f9b8ccbe988">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="86b8b3c5-517c-496b-9821-88915a51ecdf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8c3cbf71774463a7346d122e157c28df" ns3:_="">
     <xsd:import namespace="86b8b3c5-517c-496b-9821-88915a51ecdf"/>
@@ -1193,6 +1215,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C68E5401-E02F-48BB-ABBA-CA4E7B79B791}">
   <ds:schemaRefs>
@@ -1202,22 +1230,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BB1146C-31BC-4F67-BB13-7485F9CC6A56}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="86b8b3c5-517c-496b-9821-88915a51ecdf"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D193430A-6E87-4ED3-8DE5-16693E1B48D3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1233,4 +1245,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BB1146C-31BC-4F67-BB13-7485F9CC6A56}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="86b8b3c5-517c-496b-9821-88915a51ecdf"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>